<commit_message>
Mise en conformité avec nouvel arrêté RPPS (#271)
* suppression nationality extension

* rm extension nationality

* rm elements 45b6ad7f292962003dca2d8734bfece806b5adc4
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-as-dp-practitioner.xlsx
+++ b/main/ig/StructureDefinition-as-dp-practitioner.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13705" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13705" uniqueCount="1045">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-08T12:14:02+00:00</t>
+    <t>2025-10-08T12:28:03+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2725,9 +2725,6 @@
   </si>
   <si>
     <t>Often, specific identities are assigned for the qualification.</t>
-  </si>
-  <si>
-    <t>Diplome.numeroDiplome</t>
   </si>
   <si>
     <t>.playingEntity.playingRole[classCode=QUAL].id</t>
@@ -36120,22 +36117,22 @@
         <v>84</v>
       </c>
       <c r="AN242" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AO242" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AP242" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AQ242" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AR242" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AS242" t="s" s="2">
         <v>874</v>
-      </c>
-      <c r="AO242" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AP242" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AQ242" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AR242" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AS242" t="s" s="2">
-        <v>875</v>
       </c>
       <c r="AT242" t="s" s="2">
         <v>84</v>
@@ -36146,10 +36143,10 @@
     </row>
     <row r="243" hidden="true">
       <c r="A243" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B243" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C243" s="2"/>
       <c r="D243" t="s" s="2">
@@ -36175,10 +36172,10 @@
         <v>249</v>
       </c>
       <c r="L243" t="s" s="2">
+        <v>876</v>
+      </c>
+      <c r="M243" t="s" s="2">
         <v>877</v>
-      </c>
-      <c r="M243" t="s" s="2">
-        <v>878</v>
       </c>
       <c r="N243" s="2"/>
       <c r="O243" s="2"/>
@@ -36208,11 +36205,11 @@
         <v>181</v>
       </c>
       <c r="Y243" t="s" s="2">
+        <v>878</v>
+      </c>
+      <c r="Z243" t="s" s="2">
         <v>879</v>
       </c>
-      <c r="Z243" t="s" s="2">
-        <v>880</v>
-      </c>
       <c r="AA243" t="s" s="2">
         <v>84</v>
       </c>
@@ -36229,7 +36226,7 @@
         <v>84</v>
       </c>
       <c r="AF243" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="AG243" t="s" s="2">
         <v>102</v>
@@ -36253,7 +36250,7 @@
         <v>84</v>
       </c>
       <c r="AN243" t="s" s="2">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="AO243" t="s" s="2">
         <v>84</v>
@@ -36271,7 +36268,7 @@
         <v>861</v>
       </c>
       <c r="AT243" t="s" s="2">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="AU243" t="s" s="2">
         <v>84</v>
@@ -36279,10 +36276,10 @@
     </row>
     <row r="244" hidden="true">
       <c r="A244" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B244" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C244" s="2"/>
       <c r="D244" t="s" s="2">
@@ -36308,14 +36305,14 @@
         <v>269</v>
       </c>
       <c r="L244" t="s" s="2">
+        <v>883</v>
+      </c>
+      <c r="M244" t="s" s="2">
         <v>884</v>
-      </c>
-      <c r="M244" t="s" s="2">
-        <v>885</v>
       </c>
       <c r="N244" s="2"/>
       <c r="O244" t="s" s="2">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="P244" t="s" s="2">
         <v>84</v>
@@ -36364,7 +36361,7 @@
         <v>84</v>
       </c>
       <c r="AF244" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AG244" t="s" s="2">
         <v>85</v>
@@ -36403,10 +36400,10 @@
         <v>84</v>
       </c>
       <c r="AS244" t="s" s="2">
+        <v>886</v>
+      </c>
+      <c r="AT244" t="s" s="2">
         <v>887</v>
-      </c>
-      <c r="AT244" t="s" s="2">
-        <v>888</v>
       </c>
       <c r="AU244" t="s" s="2">
         <v>84</v>
@@ -36414,10 +36411,10 @@
     </row>
     <row r="245" hidden="true">
       <c r="A245" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B245" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" t="s" s="2">
@@ -36443,10 +36440,10 @@
         <v>540</v>
       </c>
       <c r="L245" t="s" s="2">
+        <v>889</v>
+      </c>
+      <c r="M245" t="s" s="2">
         <v>890</v>
-      </c>
-      <c r="M245" t="s" s="2">
-        <v>891</v>
       </c>
       <c r="N245" s="2"/>
       <c r="O245" s="2"/>
@@ -36497,7 +36494,7 @@
         <v>84</v>
       </c>
       <c r="AF245" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="AG245" t="s" s="2">
         <v>85</v>
@@ -36536,7 +36533,7 @@
         <v>84</v>
       </c>
       <c r="AS245" t="s" s="2">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="AT245" t="s" s="2">
         <v>84</v>
@@ -36547,13 +36544,13 @@
     </row>
     <row r="246" hidden="true">
       <c r="A246" t="s" s="2">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B246" t="s" s="2">
         <v>855</v>
       </c>
       <c r="C246" t="s" s="2">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D246" t="s" s="2">
         <v>84</v>
@@ -36578,7 +36575,7 @@
         <v>856</v>
       </c>
       <c r="L246" t="s" s="2">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="M246" t="s" s="2">
         <v>858</v>
@@ -36656,7 +36653,7 @@
         <v>84</v>
       </c>
       <c r="AN246" t="s" s="2">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="AO246" t="s" s="2">
         <v>84</v>
@@ -36682,7 +36679,7 @@
     </row>
     <row r="247" hidden="true">
       <c r="A247" t="s" s="2">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B247" t="s" s="2">
         <v>863</v>
@@ -36815,7 +36812,7 @@
     </row>
     <row r="248" hidden="true">
       <c r="A248" t="s" s="2">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B248" t="s" s="2">
         <v>864</v>
@@ -36946,13 +36943,13 @@
     </row>
     <row r="249">
       <c r="A249" t="s" s="2">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B249" t="s" s="2">
         <v>864</v>
       </c>
       <c r="C249" t="s" s="2">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D249" t="s" s="2">
         <v>84</v>
@@ -36974,13 +36971,13 @@
         <v>84</v>
       </c>
       <c r="K249" t="s" s="2">
+        <v>900</v>
+      </c>
+      <c r="L249" t="s" s="2">
         <v>901</v>
       </c>
-      <c r="L249" t="s" s="2">
+      <c r="M249" t="s" s="2">
         <v>902</v>
-      </c>
-      <c r="M249" t="s" s="2">
-        <v>903</v>
       </c>
       <c r="N249" s="2"/>
       <c r="O249" s="2"/>
@@ -37081,10 +37078,10 @@
     </row>
     <row r="250" hidden="true">
       <c r="A250" t="s" s="2">
+        <v>903</v>
+      </c>
+      <c r="B250" t="s" s="2">
         <v>904</v>
-      </c>
-      <c r="B250" t="s" s="2">
-        <v>905</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" t="s" s="2">
@@ -37214,10 +37211,10 @@
     </row>
     <row r="251" hidden="true">
       <c r="A251" t="s" s="2">
+        <v>905</v>
+      </c>
+      <c r="B251" t="s" s="2">
         <v>906</v>
-      </c>
-      <c r="B251" t="s" s="2">
-        <v>907</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" t="s" s="2">
@@ -37349,13 +37346,13 @@
     </row>
     <row r="252" hidden="true">
       <c r="A252" t="s" s="2">
+        <v>907</v>
+      </c>
+      <c r="B252" t="s" s="2">
+        <v>906</v>
+      </c>
+      <c r="C252" t="s" s="2">
         <v>908</v>
-      </c>
-      <c r="B252" t="s" s="2">
-        <v>907</v>
-      </c>
-      <c r="C252" t="s" s="2">
-        <v>909</v>
       </c>
       <c r="D252" t="s" s="2">
         <v>84</v>
@@ -37458,7 +37455,7 @@
         <v>84</v>
       </c>
       <c r="AN252" t="s" s="2">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="AO252" t="s" s="2">
         <v>84</v>
@@ -37484,10 +37481,10 @@
     </row>
     <row r="253" hidden="true">
       <c r="A253" t="s" s="2">
+        <v>910</v>
+      </c>
+      <c r="B253" t="s" s="2">
         <v>911</v>
-      </c>
-      <c r="B253" t="s" s="2">
-        <v>912</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" t="s" s="2">
@@ -37617,10 +37614,10 @@
     </row>
     <row r="254" hidden="true">
       <c r="A254" t="s" s="2">
+        <v>912</v>
+      </c>
+      <c r="B254" t="s" s="2">
         <v>913</v>
-      </c>
-      <c r="B254" t="s" s="2">
-        <v>914</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" t="s" s="2">
@@ -37750,10 +37747,10 @@
     </row>
     <row r="255" hidden="true">
       <c r="A255" t="s" s="2">
+        <v>914</v>
+      </c>
+      <c r="B255" t="s" s="2">
         <v>915</v>
-      </c>
-      <c r="B255" t="s" s="2">
-        <v>916</v>
       </c>
       <c r="C255" s="2"/>
       <c r="D255" t="s" s="2">
@@ -37793,7 +37790,7 @@
       </c>
       <c r="Q255" s="2"/>
       <c r="R255" t="s" s="2">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="S255" t="s" s="2">
         <v>84</v>
@@ -37885,10 +37882,10 @@
     </row>
     <row r="256" hidden="true">
       <c r="A256" t="s" s="2">
+        <v>916</v>
+      </c>
+      <c r="B256" t="s" s="2">
         <v>917</v>
-      </c>
-      <c r="B256" t="s" s="2">
-        <v>918</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" t="s" s="2">
@@ -37948,7 +37945,7 @@
       </c>
       <c r="Y256" s="2"/>
       <c r="Z256" t="s" s="2">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="AA256" t="s" s="2">
         <v>84</v>
@@ -38016,13 +38013,13 @@
     </row>
     <row r="257" hidden="true">
       <c r="A257" t="s" s="2">
+        <v>919</v>
+      </c>
+      <c r="B257" t="s" s="2">
+        <v>906</v>
+      </c>
+      <c r="C257" t="s" s="2">
         <v>920</v>
-      </c>
-      <c r="B257" t="s" s="2">
-        <v>907</v>
-      </c>
-      <c r="C257" t="s" s="2">
-        <v>921</v>
       </c>
       <c r="D257" t="s" s="2">
         <v>84</v>
@@ -38125,7 +38122,7 @@
         <v>84</v>
       </c>
       <c r="AN257" t="s" s="2">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="AO257" t="s" s="2">
         <v>84</v>
@@ -38151,10 +38148,10 @@
     </row>
     <row r="258" hidden="true">
       <c r="A258" t="s" s="2">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B258" t="s" s="2">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C258" s="2"/>
       <c r="D258" t="s" s="2">
@@ -38284,10 +38281,10 @@
     </row>
     <row r="259" hidden="true">
       <c r="A259" t="s" s="2">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B259" t="s" s="2">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" t="s" s="2">
@@ -38417,10 +38414,10 @@
     </row>
     <row r="260" hidden="true">
       <c r="A260" t="s" s="2">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B260" t="s" s="2">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" t="s" s="2">
@@ -38460,7 +38457,7 @@
       </c>
       <c r="Q260" s="2"/>
       <c r="R260" t="s" s="2">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="S260" t="s" s="2">
         <v>84</v>
@@ -38552,10 +38549,10 @@
     </row>
     <row r="261" hidden="true">
       <c r="A261" t="s" s="2">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B261" t="s" s="2">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" t="s" s="2">
@@ -38615,7 +38612,7 @@
       </c>
       <c r="Y261" s="2"/>
       <c r="Z261" t="s" s="2">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="AA261" t="s" s="2">
         <v>84</v>
@@ -38683,13 +38680,13 @@
     </row>
     <row r="262" hidden="true">
       <c r="A262" t="s" s="2">
+        <v>927</v>
+      </c>
+      <c r="B262" t="s" s="2">
+        <v>906</v>
+      </c>
+      <c r="C262" t="s" s="2">
         <v>928</v>
-      </c>
-      <c r="B262" t="s" s="2">
-        <v>907</v>
-      </c>
-      <c r="C262" t="s" s="2">
-        <v>929</v>
       </c>
       <c r="D262" t="s" s="2">
         <v>84</v>
@@ -38792,7 +38789,7 @@
         <v>84</v>
       </c>
       <c r="AN262" t="s" s="2">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="AO262" t="s" s="2">
         <v>84</v>
@@ -38818,10 +38815,10 @@
     </row>
     <row r="263" hidden="true">
       <c r="A263" t="s" s="2">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B263" t="s" s="2">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" t="s" s="2">
@@ -38951,10 +38948,10 @@
     </row>
     <row r="264" hidden="true">
       <c r="A264" t="s" s="2">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B264" t="s" s="2">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C264" s="2"/>
       <c r="D264" t="s" s="2">
@@ -39084,10 +39081,10 @@
     </row>
     <row r="265" hidden="true">
       <c r="A265" t="s" s="2">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B265" t="s" s="2">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C265" s="2"/>
       <c r="D265" t="s" s="2">
@@ -39127,7 +39124,7 @@
       </c>
       <c r="Q265" s="2"/>
       <c r="R265" t="s" s="2">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="S265" t="s" s="2">
         <v>84</v>
@@ -39219,10 +39216,10 @@
     </row>
     <row r="266" hidden="true">
       <c r="A266" t="s" s="2">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B266" t="s" s="2">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C266" s="2"/>
       <c r="D266" t="s" s="2">
@@ -39282,7 +39279,7 @@
       </c>
       <c r="Y266" s="2"/>
       <c r="Z266" t="s" s="2">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AA266" t="s" s="2">
         <v>84</v>
@@ -39350,10 +39347,10 @@
     </row>
     <row r="267" hidden="true">
       <c r="A267" t="s" s="2">
+        <v>935</v>
+      </c>
+      <c r="B267" t="s" s="2">
         <v>936</v>
-      </c>
-      <c r="B267" t="s" s="2">
-        <v>937</v>
       </c>
       <c r="C267" s="2"/>
       <c r="D267" t="s" s="2">
@@ -39393,7 +39390,7 @@
       </c>
       <c r="Q267" s="2"/>
       <c r="R267" t="s" s="2">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="S267" t="s" s="2">
         <v>84</v>
@@ -39485,10 +39482,10 @@
     </row>
     <row r="268" hidden="true">
       <c r="A268" t="s" s="2">
+        <v>938</v>
+      </c>
+      <c r="B268" t="s" s="2">
         <v>939</v>
-      </c>
-      <c r="B268" t="s" s="2">
-        <v>940</v>
       </c>
       <c r="C268" s="2"/>
       <c r="D268" t="s" s="2">
@@ -39618,7 +39615,7 @@
     </row>
     <row r="269" hidden="true">
       <c r="A269" t="s" s="2">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B269" t="s" s="2">
         <v>865</v>
@@ -39755,7 +39752,7 @@
     </row>
     <row r="270" hidden="true">
       <c r="A270" t="s" s="2">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B270" t="s" s="2">
         <v>870</v>
@@ -39879,7 +39876,7 @@
         <v>84</v>
       </c>
       <c r="AS270" t="s" s="2">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="AT270" t="s" s="2">
         <v>84</v>
@@ -39890,10 +39887,10 @@
     </row>
     <row r="271" hidden="true">
       <c r="A271" t="s" s="2">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B271" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C271" s="2"/>
       <c r="D271" t="s" s="2">
@@ -39919,10 +39916,10 @@
         <v>249</v>
       </c>
       <c r="L271" t="s" s="2">
+        <v>876</v>
+      </c>
+      <c r="M271" t="s" s="2">
         <v>877</v>
-      </c>
-      <c r="M271" t="s" s="2">
-        <v>878</v>
       </c>
       <c r="N271" s="2"/>
       <c r="O271" s="2"/>
@@ -39952,11 +39949,11 @@
         <v>181</v>
       </c>
       <c r="Y271" t="s" s="2">
+        <v>878</v>
+      </c>
+      <c r="Z271" t="s" s="2">
         <v>879</v>
       </c>
-      <c r="Z271" t="s" s="2">
-        <v>880</v>
-      </c>
       <c r="AA271" t="s" s="2">
         <v>84</v>
       </c>
@@ -39973,7 +39970,7 @@
         <v>84</v>
       </c>
       <c r="AF271" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="AG271" t="s" s="2">
         <v>102</v>
@@ -40015,7 +40012,7 @@
         <v>861</v>
       </c>
       <c r="AT271" t="s" s="2">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="AU271" t="s" s="2">
         <v>84</v>
@@ -40023,10 +40020,10 @@
     </row>
     <row r="272" hidden="true">
       <c r="A272" t="s" s="2">
+        <v>943</v>
+      </c>
+      <c r="B272" t="s" s="2">
         <v>944</v>
-      </c>
-      <c r="B272" t="s" s="2">
-        <v>945</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" t="s" s="2">
@@ -40156,10 +40153,10 @@
     </row>
     <row r="273" hidden="true">
       <c r="A273" t="s" s="2">
+        <v>945</v>
+      </c>
+      <c r="B273" t="s" s="2">
         <v>946</v>
-      </c>
-      <c r="B273" t="s" s="2">
-        <v>947</v>
       </c>
       <c r="C273" s="2"/>
       <c r="D273" t="s" s="2">
@@ -40291,10 +40288,10 @@
     </row>
     <row r="274" hidden="true">
       <c r="A274" t="s" s="2">
+        <v>947</v>
+      </c>
+      <c r="B274" t="s" s="2">
         <v>948</v>
-      </c>
-      <c r="B274" t="s" s="2">
-        <v>949</v>
       </c>
       <c r="C274" s="2"/>
       <c r="D274" t="s" s="2">
@@ -40426,13 +40423,13 @@
     </row>
     <row r="275">
       <c r="A275" t="s" s="2">
+        <v>949</v>
+      </c>
+      <c r="B275" t="s" s="2">
+        <v>948</v>
+      </c>
+      <c r="C275" t="s" s="2">
         <v>950</v>
-      </c>
-      <c r="B275" t="s" s="2">
-        <v>949</v>
-      </c>
-      <c r="C275" t="s" s="2">
-        <v>951</v>
       </c>
       <c r="D275" t="s" s="2">
         <v>84</v>
@@ -40495,7 +40492,7 @@
       </c>
       <c r="Y275" s="2"/>
       <c r="Z275" t="s" s="2">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="AA275" t="s" s="2">
         <v>84</v>
@@ -40563,13 +40560,13 @@
     </row>
     <row r="276">
       <c r="A276" t="s" s="2">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B276" t="s" s="2">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C276" t="s" s="2">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D276" t="s" s="2">
         <v>84</v>
@@ -40632,7 +40629,7 @@
       </c>
       <c r="Y276" s="2"/>
       <c r="Z276" t="s" s="2">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="AA276" t="s" s="2">
         <v>84</v>
@@ -40700,10 +40697,10 @@
     </row>
     <row r="277" hidden="true">
       <c r="A277" t="s" s="2">
+        <v>954</v>
+      </c>
+      <c r="B277" t="s" s="2">
         <v>955</v>
-      </c>
-      <c r="B277" t="s" s="2">
-        <v>956</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" t="s" s="2">
@@ -40837,10 +40834,10 @@
     </row>
     <row r="278" hidden="true">
       <c r="A278" t="s" s="2">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B278" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C278" s="2"/>
       <c r="D278" t="s" s="2">
@@ -40866,14 +40863,14 @@
         <v>269</v>
       </c>
       <c r="L278" t="s" s="2">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="M278" t="s" s="2">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="N278" s="2"/>
       <c r="O278" t="s" s="2">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="P278" t="s" s="2">
         <v>84</v>
@@ -40922,7 +40919,7 @@
         <v>84</v>
       </c>
       <c r="AF278" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AG278" t="s" s="2">
         <v>85</v>
@@ -40961,10 +40958,10 @@
         <v>84</v>
       </c>
       <c r="AS278" t="s" s="2">
+        <v>886</v>
+      </c>
+      <c r="AT278" t="s" s="2">
         <v>887</v>
-      </c>
-      <c r="AT278" t="s" s="2">
-        <v>888</v>
       </c>
       <c r="AU278" t="s" s="2">
         <v>84</v>
@@ -40972,10 +40969,10 @@
     </row>
     <row r="279" hidden="true">
       <c r="A279" t="s" s="2">
+        <v>958</v>
+      </c>
+      <c r="B279" t="s" s="2">
         <v>959</v>
-      </c>
-      <c r="B279" t="s" s="2">
-        <v>960</v>
       </c>
       <c r="C279" s="2"/>
       <c r="D279" t="s" s="2">
@@ -41105,10 +41102,10 @@
     </row>
     <row r="280" hidden="true">
       <c r="A280" t="s" s="2">
+        <v>960</v>
+      </c>
+      <c r="B280" t="s" s="2">
         <v>961</v>
-      </c>
-      <c r="B280" t="s" s="2">
-        <v>962</v>
       </c>
       <c r="C280" s="2"/>
       <c r="D280" t="s" s="2">
@@ -41240,10 +41237,10 @@
     </row>
     <row r="281" hidden="true">
       <c r="A281" t="s" s="2">
+        <v>962</v>
+      </c>
+      <c r="B281" t="s" s="2">
         <v>963</v>
-      </c>
-      <c r="B281" t="s" s="2">
-        <v>964</v>
       </c>
       <c r="C281" s="2"/>
       <c r="D281" t="s" s="2">
@@ -41269,7 +41266,7 @@
         <v>276</v>
       </c>
       <c r="L281" t="s" s="2">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="M281" t="s" s="2">
         <v>278</v>
@@ -41349,7 +41346,7 @@
         <v>84</v>
       </c>
       <c r="AN281" t="s" s="2">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="AO281" t="s" s="2">
         <v>84</v>
@@ -41375,10 +41372,10 @@
     </row>
     <row r="282" hidden="true">
       <c r="A282" t="s" s="2">
+        <v>966</v>
+      </c>
+      <c r="B282" t="s" s="2">
         <v>967</v>
-      </c>
-      <c r="B282" t="s" s="2">
-        <v>968</v>
       </c>
       <c r="C282" s="2"/>
       <c r="D282" t="s" s="2">
@@ -41404,7 +41401,7 @@
         <v>276</v>
       </c>
       <c r="L282" t="s" s="2">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="M282" t="s" s="2">
         <v>288</v>
@@ -41486,7 +41483,7 @@
         <v>84</v>
       </c>
       <c r="AN282" t="s" s="2">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="AO282" t="s" s="2">
         <v>84</v>
@@ -41512,10 +41509,10 @@
     </row>
     <row r="283" hidden="true">
       <c r="A283" t="s" s="2">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B283" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C283" s="2"/>
       <c r="D283" t="s" s="2">
@@ -41538,13 +41535,13 @@
         <v>84</v>
       </c>
       <c r="K283" t="s" s="2">
+        <v>971</v>
+      </c>
+      <c r="L283" t="s" s="2">
         <v>972</v>
       </c>
-      <c r="L283" t="s" s="2">
-        <v>973</v>
-      </c>
       <c r="M283" t="s" s="2">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="N283" s="2"/>
       <c r="O283" s="2"/>
@@ -41595,7 +41592,7 @@
         <v>84</v>
       </c>
       <c r="AF283" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="AG283" t="s" s="2">
         <v>85</v>
@@ -41619,7 +41616,7 @@
         <v>84</v>
       </c>
       <c r="AN283" t="s" s="2">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="AO283" t="s" s="2">
         <v>84</v>
@@ -41634,7 +41631,7 @@
         <v>84</v>
       </c>
       <c r="AS283" t="s" s="2">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="AT283" t="s" s="2">
         <v>84</v>
@@ -41645,13 +41642,13 @@
     </row>
     <row r="284" hidden="true">
       <c r="A284" t="s" s="2">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B284" t="s" s="2">
         <v>855</v>
       </c>
       <c r="C284" t="s" s="2">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D284" t="s" s="2">
         <v>84</v>
@@ -41676,7 +41673,7 @@
         <v>856</v>
       </c>
       <c r="L284" t="s" s="2">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="M284" t="s" s="2">
         <v>858</v>
@@ -41780,7 +41777,7 @@
     </row>
     <row r="285" hidden="true">
       <c r="A285" t="s" s="2">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B285" t="s" s="2">
         <v>863</v>
@@ -41913,7 +41910,7 @@
     </row>
     <row r="286" hidden="true">
       <c r="A286" t="s" s="2">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B286" t="s" s="2">
         <v>864</v>
@@ -42048,7 +42045,7 @@
     </row>
     <row r="287" hidden="true">
       <c r="A287" t="s" s="2">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B287" t="s" s="2">
         <v>865</v>
@@ -42185,7 +42182,7 @@
     </row>
     <row r="288" hidden="true">
       <c r="A288" t="s" s="2">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B288" t="s" s="2">
         <v>870</v>
@@ -42309,7 +42306,7 @@
         <v>84</v>
       </c>
       <c r="AS288" t="s" s="2">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="AT288" t="s" s="2">
         <v>84</v>
@@ -42320,10 +42317,10 @@
     </row>
     <row r="289" hidden="true">
       <c r="A289" t="s" s="2">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B289" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C289" s="2"/>
       <c r="D289" t="s" s="2">
@@ -42349,10 +42346,10 @@
         <v>249</v>
       </c>
       <c r="L289" t="s" s="2">
+        <v>876</v>
+      </c>
+      <c r="M289" t="s" s="2">
         <v>877</v>
-      </c>
-      <c r="M289" t="s" s="2">
-        <v>878</v>
       </c>
       <c r="N289" s="2"/>
       <c r="O289" s="2"/>
@@ -42382,11 +42379,11 @@
         <v>181</v>
       </c>
       <c r="Y289" t="s" s="2">
+        <v>878</v>
+      </c>
+      <c r="Z289" t="s" s="2">
         <v>879</v>
       </c>
-      <c r="Z289" t="s" s="2">
-        <v>880</v>
-      </c>
       <c r="AA289" t="s" s="2">
         <v>84</v>
       </c>
@@ -42403,7 +42400,7 @@
         <v>84</v>
       </c>
       <c r="AF289" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="AG289" t="s" s="2">
         <v>102</v>
@@ -42445,7 +42442,7 @@
         <v>861</v>
       </c>
       <c r="AT289" t="s" s="2">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="AU289" t="s" s="2">
         <v>84</v>
@@ -42453,10 +42450,10 @@
     </row>
     <row r="290" hidden="true">
       <c r="A290" t="s" s="2">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B290" t="s" s="2">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C290" s="2"/>
       <c r="D290" t="s" s="2">
@@ -42586,10 +42583,10 @@
     </row>
     <row r="291" hidden="true">
       <c r="A291" t="s" s="2">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B291" t="s" s="2">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" t="s" s="2">
@@ -42721,10 +42718,10 @@
     </row>
     <row r="292" hidden="true">
       <c r="A292" t="s" s="2">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B292" t="s" s="2">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C292" s="2"/>
       <c r="D292" t="s" s="2">
@@ -42856,13 +42853,13 @@
     </row>
     <row r="293">
       <c r="A293" t="s" s="2">
+        <v>985</v>
+      </c>
+      <c r="B293" t="s" s="2">
+        <v>948</v>
+      </c>
+      <c r="C293" t="s" s="2">
         <v>986</v>
-      </c>
-      <c r="B293" t="s" s="2">
-        <v>949</v>
-      </c>
-      <c r="C293" t="s" s="2">
-        <v>987</v>
       </c>
       <c r="D293" t="s" s="2">
         <v>84</v>
@@ -42887,7 +42884,7 @@
         <v>169</v>
       </c>
       <c r="L293" t="s" s="2">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="M293" t="s" s="2">
         <v>459</v>
@@ -42925,7 +42922,7 @@
       </c>
       <c r="Y293" s="2"/>
       <c r="Z293" t="s" s="2">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="AA293" t="s" s="2">
         <v>84</v>
@@ -42961,7 +42958,7 @@
         <v>84</v>
       </c>
       <c r="AL293" t="s" s="2">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="AM293" t="s" s="2">
         <v>84</v>
@@ -42993,10 +42990,10 @@
     </row>
     <row r="294">
       <c r="A294" t="s" s="2">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B294" t="s" s="2">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C294" t="s" s="2">
         <v>361</v>
@@ -43024,7 +43021,7 @@
         <v>169</v>
       </c>
       <c r="L294" t="s" s="2">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="M294" t="s" s="2">
         <v>459</v>
@@ -43098,7 +43095,7 @@
         <v>84</v>
       </c>
       <c r="AL294" t="s" s="2">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="AM294" t="s" s="2">
         <v>84</v>
@@ -43130,10 +43127,10 @@
     </row>
     <row r="295" hidden="true">
       <c r="A295" t="s" s="2">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B295" t="s" s="2">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C295" s="2"/>
       <c r="D295" t="s" s="2">
@@ -43267,10 +43264,10 @@
     </row>
     <row r="296">
       <c r="A296" t="s" s="2">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B296" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" t="s" s="2">
@@ -43296,14 +43293,14 @@
         <v>269</v>
       </c>
       <c r="L296" t="s" s="2">
+        <v>883</v>
+      </c>
+      <c r="M296" t="s" s="2">
         <v>884</v>
-      </c>
-      <c r="M296" t="s" s="2">
-        <v>885</v>
       </c>
       <c r="N296" s="2"/>
       <c r="O296" t="s" s="2">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="P296" t="s" s="2">
         <v>84</v>
@@ -43352,7 +43349,7 @@
         <v>84</v>
       </c>
       <c r="AF296" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AG296" t="s" s="2">
         <v>85</v>
@@ -43391,10 +43388,10 @@
         <v>84</v>
       </c>
       <c r="AS296" t="s" s="2">
+        <v>886</v>
+      </c>
+      <c r="AT296" t="s" s="2">
         <v>887</v>
-      </c>
-      <c r="AT296" t="s" s="2">
-        <v>888</v>
       </c>
       <c r="AU296" t="s" s="2">
         <v>84</v>
@@ -43402,10 +43399,10 @@
     </row>
     <row r="297" hidden="true">
       <c r="A297" t="s" s="2">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B297" t="s" s="2">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" t="s" s="2">
@@ -43535,10 +43532,10 @@
     </row>
     <row r="298" hidden="true">
       <c r="A298" t="s" s="2">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B298" t="s" s="2">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" t="s" s="2">
@@ -43670,10 +43667,10 @@
     </row>
     <row r="299" hidden="true">
       <c r="A299" t="s" s="2">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B299" t="s" s="2">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C299" s="2"/>
       <c r="D299" t="s" s="2">
@@ -43699,7 +43696,7 @@
         <v>276</v>
       </c>
       <c r="L299" t="s" s="2">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="M299" t="s" s="2">
         <v>278</v>
@@ -43773,7 +43770,7 @@
         <v>84</v>
       </c>
       <c r="AL299" t="s" s="2">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="AM299" t="s" s="2">
         <v>84</v>
@@ -43805,10 +43802,10 @@
     </row>
     <row r="300" hidden="true">
       <c r="A300" t="s" s="2">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B300" t="s" s="2">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C300" s="2"/>
       <c r="D300" t="s" s="2">
@@ -43834,7 +43831,7 @@
         <v>276</v>
       </c>
       <c r="L300" t="s" s="2">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="M300" t="s" s="2">
         <v>288</v>
@@ -43910,7 +43907,7 @@
         <v>84</v>
       </c>
       <c r="AL300" t="s" s="2">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="AM300" t="s" s="2">
         <v>84</v>
@@ -43942,10 +43939,10 @@
     </row>
     <row r="301" hidden="true">
       <c r="A301" t="s" s="2">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B301" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C301" s="2"/>
       <c r="D301" t="s" s="2">
@@ -43971,10 +43968,10 @@
         <v>540</v>
       </c>
       <c r="L301" t="s" s="2">
+        <v>889</v>
+      </c>
+      <c r="M301" t="s" s="2">
         <v>890</v>
-      </c>
-      <c r="M301" t="s" s="2">
-        <v>891</v>
       </c>
       <c r="N301" s="2"/>
       <c r="O301" s="2"/>
@@ -44025,7 +44022,7 @@
         <v>84</v>
       </c>
       <c r="AF301" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="AG301" t="s" s="2">
         <v>85</v>
@@ -44064,7 +44061,7 @@
         <v>84</v>
       </c>
       <c r="AS301" t="s" s="2">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="AT301" t="s" s="2">
         <v>84</v>
@@ -44075,13 +44072,13 @@
     </row>
     <row r="302" hidden="true">
       <c r="A302" t="s" s="2">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B302" t="s" s="2">
         <v>855</v>
       </c>
       <c r="C302" t="s" s="2">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="D302" t="s" s="2">
         <v>84</v>
@@ -44106,7 +44103,7 @@
         <v>856</v>
       </c>
       <c r="L302" t="s" s="2">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="M302" t="s" s="2">
         <v>858</v>
@@ -44210,7 +44207,7 @@
     </row>
     <row r="303" hidden="true">
       <c r="A303" t="s" s="2">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B303" t="s" s="2">
         <v>863</v>
@@ -44343,7 +44340,7 @@
     </row>
     <row r="304" hidden="true">
       <c r="A304" t="s" s="2">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B304" t="s" s="2">
         <v>864</v>
@@ -44478,7 +44475,7 @@
     </row>
     <row r="305" hidden="true">
       <c r="A305" t="s" s="2">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B305" t="s" s="2">
         <v>865</v>
@@ -44615,7 +44612,7 @@
     </row>
     <row r="306" hidden="true">
       <c r="A306" t="s" s="2">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B306" t="s" s="2">
         <v>870</v>
@@ -44739,7 +44736,7 @@
         <v>84</v>
       </c>
       <c r="AS306" t="s" s="2">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="AT306" t="s" s="2">
         <v>84</v>
@@ -44750,10 +44747,10 @@
     </row>
     <row r="307" hidden="true">
       <c r="A307" t="s" s="2">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B307" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C307" s="2"/>
       <c r="D307" t="s" s="2">
@@ -44779,10 +44776,10 @@
         <v>249</v>
       </c>
       <c r="L307" t="s" s="2">
+        <v>876</v>
+      </c>
+      <c r="M307" t="s" s="2">
         <v>877</v>
-      </c>
-      <c r="M307" t="s" s="2">
-        <v>878</v>
       </c>
       <c r="N307" s="2"/>
       <c r="O307" s="2"/>
@@ -44812,11 +44809,11 @@
         <v>181</v>
       </c>
       <c r="Y307" t="s" s="2">
+        <v>878</v>
+      </c>
+      <c r="Z307" t="s" s="2">
         <v>879</v>
       </c>
-      <c r="Z307" t="s" s="2">
-        <v>880</v>
-      </c>
       <c r="AA307" t="s" s="2">
         <v>84</v>
       </c>
@@ -44833,7 +44830,7 @@
         <v>84</v>
       </c>
       <c r="AF307" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="AG307" t="s" s="2">
         <v>102</v>
@@ -44848,7 +44845,7 @@
         <v>114</v>
       </c>
       <c r="AK307" t="s" s="2">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="AL307" t="s" s="2">
         <v>84</v>
@@ -44875,7 +44872,7 @@
         <v>861</v>
       </c>
       <c r="AT307" t="s" s="2">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="AU307" t="s" s="2">
         <v>84</v>
@@ -44883,10 +44880,10 @@
     </row>
     <row r="308" hidden="true">
       <c r="A308" t="s" s="2">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B308" t="s" s="2">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C308" s="2"/>
       <c r="D308" t="s" s="2">
@@ -45016,10 +45013,10 @@
     </row>
     <row r="309" hidden="true">
       <c r="A309" t="s" s="2">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B309" t="s" s="2">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C309" s="2"/>
       <c r="D309" t="s" s="2">
@@ -45151,10 +45148,10 @@
     </row>
     <row r="310" hidden="true">
       <c r="A310" t="s" s="2">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B310" t="s" s="2">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C310" s="2"/>
       <c r="D310" t="s" s="2">
@@ -45286,13 +45283,13 @@
     </row>
     <row r="311">
       <c r="A311" t="s" s="2">
+        <v>1016</v>
+      </c>
+      <c r="B311" t="s" s="2">
+        <v>948</v>
+      </c>
+      <c r="C311" t="s" s="2">
         <v>1017</v>
-      </c>
-      <c r="B311" t="s" s="2">
-        <v>949</v>
-      </c>
-      <c r="C311" t="s" s="2">
-        <v>1018</v>
       </c>
       <c r="D311" t="s" s="2">
         <v>84</v>
@@ -45317,7 +45314,7 @@
         <v>169</v>
       </c>
       <c r="L311" t="s" s="2">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="M311" t="s" s="2">
         <v>459</v>
@@ -45355,7 +45352,7 @@
       </c>
       <c r="Y311" s="2"/>
       <c r="Z311" t="s" s="2">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="AA311" t="s" s="2">
         <v>84</v>
@@ -45388,7 +45385,7 @@
         <v>114</v>
       </c>
       <c r="AK311" t="s" s="2">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="AL311" t="s" s="2">
         <v>84</v>
@@ -45423,13 +45420,13 @@
     </row>
     <row r="312">
       <c r="A312" t="s" s="2">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B312" t="s" s="2">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C312" t="s" s="2">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="D312" t="s" s="2">
         <v>84</v>
@@ -45454,7 +45451,7 @@
         <v>169</v>
       </c>
       <c r="L312" t="s" s="2">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="M312" t="s" s="2">
         <v>459</v>
@@ -45492,7 +45489,7 @@
       </c>
       <c r="Y312" s="2"/>
       <c r="Z312" t="s" s="2">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="AA312" t="s" s="2">
         <v>84</v>
@@ -45560,10 +45557,10 @@
     </row>
     <row r="313" hidden="true">
       <c r="A313" t="s" s="2">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B313" t="s" s="2">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C313" s="2"/>
       <c r="D313" t="s" s="2">
@@ -45697,10 +45694,10 @@
     </row>
     <row r="314" hidden="true">
       <c r="A314" t="s" s="2">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B314" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C314" s="2"/>
       <c r="D314" t="s" s="2">
@@ -45726,14 +45723,14 @@
         <v>269</v>
       </c>
       <c r="L314" t="s" s="2">
+        <v>883</v>
+      </c>
+      <c r="M314" t="s" s="2">
         <v>884</v>
-      </c>
-      <c r="M314" t="s" s="2">
-        <v>885</v>
       </c>
       <c r="N314" s="2"/>
       <c r="O314" t="s" s="2">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="P314" t="s" s="2">
         <v>84</v>
@@ -45782,7 +45779,7 @@
         <v>84</v>
       </c>
       <c r="AF314" t="s" s="2">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AG314" t="s" s="2">
         <v>85</v>
@@ -45821,10 +45818,10 @@
         <v>84</v>
       </c>
       <c r="AS314" t="s" s="2">
+        <v>886</v>
+      </c>
+      <c r="AT314" t="s" s="2">
         <v>887</v>
-      </c>
-      <c r="AT314" t="s" s="2">
-        <v>888</v>
       </c>
       <c r="AU314" t="s" s="2">
         <v>84</v>
@@ -45832,10 +45829,10 @@
     </row>
     <row r="315" hidden="true">
       <c r="A315" t="s" s="2">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B315" t="s" s="2">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C315" s="2"/>
       <c r="D315" t="s" s="2">
@@ -45965,10 +45962,10 @@
     </row>
     <row r="316" hidden="true">
       <c r="A316" t="s" s="2">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B316" t="s" s="2">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C316" s="2"/>
       <c r="D316" t="s" s="2">
@@ -46100,10 +46097,10 @@
     </row>
     <row r="317" hidden="true">
       <c r="A317" t="s" s="2">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B317" t="s" s="2">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C317" s="2"/>
       <c r="D317" t="s" s="2">
@@ -46129,7 +46126,7 @@
         <v>276</v>
       </c>
       <c r="L317" t="s" s="2">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="M317" t="s" s="2">
         <v>278</v>
@@ -46200,7 +46197,7 @@
         <v>114</v>
       </c>
       <c r="AK317" t="s" s="2">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="AL317" t="s" s="2">
         <v>84</v>
@@ -46235,10 +46232,10 @@
     </row>
     <row r="318" hidden="true">
       <c r="A318" t="s" s="2">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B318" t="s" s="2">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C318" s="2"/>
       <c r="D318" t="s" s="2">
@@ -46264,7 +46261,7 @@
         <v>276</v>
       </c>
       <c r="L318" t="s" s="2">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="M318" t="s" s="2">
         <v>288</v>
@@ -46337,7 +46334,7 @@
         <v>114</v>
       </c>
       <c r="AK318" t="s" s="2">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="AL318" t="s" s="2">
         <v>84</v>
@@ -46372,10 +46369,10 @@
     </row>
     <row r="319" hidden="true">
       <c r="A319" t="s" s="2">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B319" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C319" s="2"/>
       <c r="D319" t="s" s="2">
@@ -46401,10 +46398,10 @@
         <v>540</v>
       </c>
       <c r="L319" t="s" s="2">
+        <v>889</v>
+      </c>
+      <c r="M319" t="s" s="2">
         <v>890</v>
-      </c>
-      <c r="M319" t="s" s="2">
-        <v>891</v>
       </c>
       <c r="N319" s="2"/>
       <c r="O319" s="2"/>
@@ -46455,7 +46452,7 @@
         <v>84</v>
       </c>
       <c r="AF319" t="s" s="2">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="AG319" t="s" s="2">
         <v>85</v>
@@ -46494,7 +46491,7 @@
         <v>84</v>
       </c>
       <c r="AS319" t="s" s="2">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="AT319" t="s" s="2">
         <v>84</v>
@@ -46505,10 +46502,10 @@
     </row>
     <row r="320">
       <c r="A320" t="s" s="2">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B320" t="s" s="2">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C320" s="2"/>
       <c r="D320" t="s" s="2">
@@ -46531,19 +46528,19 @@
         <v>84</v>
       </c>
       <c r="K320" t="s" s="2">
+        <v>1036</v>
+      </c>
+      <c r="L320" t="s" s="2">
         <v>1037</v>
       </c>
-      <c r="L320" t="s" s="2">
+      <c r="M320" t="s" s="2">
         <v>1038</v>
       </c>
-      <c r="M320" t="s" s="2">
+      <c r="N320" t="s" s="2">
         <v>1039</v>
       </c>
-      <c r="N320" t="s" s="2">
+      <c r="O320" t="s" s="2">
         <v>1040</v>
-      </c>
-      <c r="O320" t="s" s="2">
-        <v>1041</v>
       </c>
       <c r="P320" t="s" s="2">
         <v>84</v>
@@ -46572,7 +46569,7 @@
       </c>
       <c r="Y320" s="2"/>
       <c r="Z320" t="s" s="2">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="AA320" t="s" s="2">
         <v>84</v>
@@ -46590,7 +46587,7 @@
         <v>84</v>
       </c>
       <c r="AF320" t="s" s="2">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="AG320" t="s" s="2">
         <v>85</v>
@@ -46626,13 +46623,13 @@
         <v>84</v>
       </c>
       <c r="AR320" t="s" s="2">
+        <v>1042</v>
+      </c>
+      <c r="AS320" t="s" s="2">
         <v>1043</v>
       </c>
-      <c r="AS320" t="s" s="2">
+      <c r="AT320" t="s" s="2">
         <v>1044</v>
-      </c>
-      <c r="AT320" t="s" s="2">
-        <v>1045</v>
       </c>
       <c r="AU320" t="s" s="2">
         <v>84</v>

</xml_diff>